<commit_message>
#Update cr site index.html #Update Expenses.xslx
</commit_message>
<xml_diff>
--- a/portfolio/expApp/Expenses.xlsx
+++ b/portfolio/expApp/Expenses.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\expense\expapp\git\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\chongraen\portfolio\expapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2911,7 +2911,7 @@
   <dimension ref="A1:K1246"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3491,13 +3491,13 @@
       </c>
       <c r="C17" s="35">
         <f t="shared" si="0"/>
-        <v>2848.37</v>
+        <v>3050</v>
       </c>
       <c r="D17" s="36">
         <v>0</v>
       </c>
       <c r="E17" s="37">
-        <v>201.63</v>
+        <v>0</v>
       </c>
       <c r="F17" s="38">
         <v>0</v>
@@ -3508,7 +3508,9 @@
       <c r="H17" s="33">
         <v>200</v>
       </c>
-      <c r="I17" s="40"/>
+      <c r="I17" s="40">
+        <v>0</v>
+      </c>
       <c r="J17" s="41">
         <f>'Expenses Details'!B17</f>
         <v>0</v>
@@ -3518,17 +3520,31 @@
       <c r="A18" s="95">
         <v>43344</v>
       </c>
-      <c r="B18" s="29"/>
+      <c r="B18" s="29">
+        <v>3500</v>
+      </c>
       <c r="C18" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D18" s="36"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="40"/>
+        <v>3098.37</v>
+      </c>
+      <c r="D18" s="36">
+        <v>0</v>
+      </c>
+      <c r="E18" s="37">
+        <v>201.63</v>
+      </c>
+      <c r="F18" s="38">
+        <v>0</v>
+      </c>
+      <c r="G18" s="39">
+        <v>0</v>
+      </c>
+      <c r="H18" s="33">
+        <v>200</v>
+      </c>
+      <c r="I18" s="40">
+        <v>0</v>
+      </c>
       <c r="J18" s="41">
         <f>'Expenses Details'!B18</f>
         <v>0</v>
@@ -3538,17 +3554,31 @@
       <c r="A19" s="95">
         <v>43374</v>
       </c>
-      <c r="B19" s="29"/>
+      <c r="B19" s="29">
+        <v>3500</v>
+      </c>
       <c r="C19" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D19" s="36"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="33"/>
-      <c r="I19" s="40"/>
+        <v>2748.37</v>
+      </c>
+      <c r="D19" s="36">
+        <v>0</v>
+      </c>
+      <c r="E19" s="37">
+        <v>201.63</v>
+      </c>
+      <c r="F19" s="38">
+        <v>0</v>
+      </c>
+      <c r="G19" s="39">
+        <v>0</v>
+      </c>
+      <c r="H19" s="33">
+        <v>200</v>
+      </c>
+      <c r="I19" s="40">
+        <v>350</v>
+      </c>
       <c r="J19" s="41">
         <f>'Expenses Details'!B19</f>
         <v>0</v>
@@ -3558,17 +3588,31 @@
       <c r="A20" s="95">
         <v>43405</v>
       </c>
-      <c r="B20" s="29"/>
+      <c r="B20" s="29">
+        <v>3500</v>
+      </c>
       <c r="C20" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D20" s="36"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="38"/>
-      <c r="G20" s="39"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="40"/>
+        <v>2748.37</v>
+      </c>
+      <c r="D20" s="36">
+        <v>0</v>
+      </c>
+      <c r="E20" s="37">
+        <v>201.63</v>
+      </c>
+      <c r="F20" s="38">
+        <v>0</v>
+      </c>
+      <c r="G20" s="39">
+        <v>0</v>
+      </c>
+      <c r="H20" s="33">
+        <v>200</v>
+      </c>
+      <c r="I20" s="40">
+        <v>350</v>
+      </c>
       <c r="J20" s="41">
         <f>'Expenses Details'!B20</f>
         <v>0</v>
@@ -3578,17 +3622,31 @@
       <c r="A21" s="95">
         <v>43435</v>
       </c>
-      <c r="B21" s="29"/>
+      <c r="B21" s="29">
+        <v>3500</v>
+      </c>
       <c r="C21" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D21" s="36"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="38"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="40"/>
+        <v>2448.37</v>
+      </c>
+      <c r="D21" s="36">
+        <v>300</v>
+      </c>
+      <c r="E21" s="37">
+        <v>201.63</v>
+      </c>
+      <c r="F21" s="38">
+        <v>0</v>
+      </c>
+      <c r="G21" s="39">
+        <v>0</v>
+      </c>
+      <c r="H21" s="33">
+        <v>200</v>
+      </c>
+      <c r="I21" s="40">
+        <v>350</v>
+      </c>
       <c r="J21" s="41">
         <f>'Expenses Details'!B21</f>
         <v>0</v>
@@ -25657,10 +25715,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -25701,11 +25759,11 @@
       </c>
       <c r="C2" s="28">
         <f>B2-D2</f>
-        <v>28512.696999999996</v>
+        <v>27847.317999999999</v>
       </c>
       <c r="D2" s="29">
         <f>SUM(Dashboard!E2:E1048576)*1.1</f>
-        <v>2439.7230000000004</v>
+        <v>3105.1020000000008</v>
       </c>
       <c r="G2" s="27" t="s">
         <v>1</v>
@@ -25769,11 +25827,11 @@
       </c>
       <c r="C4" s="28">
         <f>B4-D4</f>
-        <v>13600</v>
+        <v>13300</v>
       </c>
       <c r="D4" s="29">
         <f>SUM(Dashboard!D2:D1048576)</f>
-        <v>2400</v>
+        <v>2700</v>
       </c>
       <c r="G4" s="27" t="s">
         <v>23</v>
@@ -25898,6 +25956,12 @@
       <c r="D10" s="94">
         <f>D5</f>
         <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3">
+      <c r="C19" s="22">
+        <f>27910.97-C2</f>
+        <v>63.652000000001863</v>
       </c>
     </row>
   </sheetData>
@@ -39620,7 +39684,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D79"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A55" workbookViewId="0">
       <selection activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>

</xml_diff>